<commit_message>
add ID button works
</commit_message>
<xml_diff>
--- a/Data/register.xlsx
+++ b/Data/register.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
   <si>
     <t>FirstName</t>
   </si>
@@ -85,6 +85,252 @@
   </si>
   <si>
     <t>nTQfg3UrNO@gmail.com</t>
+  </si>
+  <si>
+    <t>Dp6gC2e51J@gmail.com</t>
+  </si>
+  <si>
+    <t>Sdapp2u9Pe@gmail.com</t>
+  </si>
+  <si>
+    <t>giMvdbnHD9@gmail.com</t>
+  </si>
+  <si>
+    <t>0rJFXpBEfk@gmail.com</t>
+  </si>
+  <si>
+    <t>vR0czRjqM2@gmail.com</t>
+  </si>
+  <si>
+    <t>kdDJF2thWz@gmail.com</t>
+  </si>
+  <si>
+    <t>vgahN2T9Js@gmail.com</t>
+  </si>
+  <si>
+    <t>oWjJWltZWT@gmail.com</t>
+  </si>
+  <si>
+    <t>pA2xNe4apf@gmail.com</t>
+  </si>
+  <si>
+    <t>9NVfzmWM2f@gmail.com</t>
+  </si>
+  <si>
+    <t>rALoNUqR6Y@gmail.com</t>
+  </si>
+  <si>
+    <t>q2a9Hp5Bw1@gmail.com</t>
+  </si>
+  <si>
+    <t>6zckwqcelI@gmail.com</t>
+  </si>
+  <si>
+    <t>3obJolfftg@gmail.com</t>
+  </si>
+  <si>
+    <t>0XtXSNei6z@gmail.com</t>
+  </si>
+  <si>
+    <t>zk2DnAP5TC@gmail.com</t>
+  </si>
+  <si>
+    <t>sd4chqceXy@gmail.com</t>
+  </si>
+  <si>
+    <t>qbnqkbQMU8@gmail.com</t>
+  </si>
+  <si>
+    <t>LvFvclcZfj@gmail.com</t>
+  </si>
+  <si>
+    <t>xMrVMayAhN@gmail.com</t>
+  </si>
+  <si>
+    <t>9gaurZEI5L@gmail.com</t>
+  </si>
+  <si>
+    <t>mNmDi3s9Q5@gmail.com</t>
+  </si>
+  <si>
+    <t>QBN00oM2Ow@gmail.com</t>
+  </si>
+  <si>
+    <t>U3T5gN7reh@gmail.com</t>
+  </si>
+  <si>
+    <t>s29TfWs2w1@gmail.com</t>
+  </si>
+  <si>
+    <t>pPrrYTuQUs@gmail.com</t>
+  </si>
+  <si>
+    <t>ZGmrPJgDML@gmail.com</t>
+  </si>
+  <si>
+    <t>oHhOCLFibX@gmail.com</t>
+  </si>
+  <si>
+    <t>EKzWR01yCL@gmail.com</t>
+  </si>
+  <si>
+    <t>WFwTFS0EhQ@gmail.com</t>
+  </si>
+  <si>
+    <t>lIIibza9oJ@gmail.com</t>
+  </si>
+  <si>
+    <t>wMVCMJOuZe@gmail.com</t>
+  </si>
+  <si>
+    <t>1BYx875pMo@gmail.com</t>
+  </si>
+  <si>
+    <t>RMx58gFGsr@gmail.com</t>
+  </si>
+  <si>
+    <t>5BfWyMZ9Mn@gmail.com</t>
+  </si>
+  <si>
+    <t>m8ERtndpfg@gmail.com</t>
+  </si>
+  <si>
+    <t>JwGPJTNXky@gmail.com</t>
+  </si>
+  <si>
+    <t>qgv7SQ26c4@gmail.com</t>
+  </si>
+  <si>
+    <t>t9Aql6FS74@gmail.com</t>
+  </si>
+  <si>
+    <t>kvcMPabBhY@gmail.com</t>
+  </si>
+  <si>
+    <t>TfzvkDZl5y@gmail.com</t>
+  </si>
+  <si>
+    <t>TPQlPW8NoC@gmail.com</t>
+  </si>
+  <si>
+    <t>R4HmuMKoag@gmail.com</t>
+  </si>
+  <si>
+    <t>vNDjnS9FUK@gmail.com</t>
+  </si>
+  <si>
+    <t>I2xQydGosu@gmail.com</t>
+  </si>
+  <si>
+    <t>JrhBaeGT7K@gmail.com</t>
+  </si>
+  <si>
+    <t>sFk93Ihizx@gmail.com</t>
+  </si>
+  <si>
+    <t>5rYBEFFQ2r@gmail.com</t>
+  </si>
+  <si>
+    <t>x2BCgAq7LN@gmail.com</t>
+  </si>
+  <si>
+    <t>BbqaumEaNB@gmail.com</t>
+  </si>
+  <si>
+    <t>tnXykr9cc4@gmail.com</t>
+  </si>
+  <si>
+    <t>zibyZzJw2h@gmail.com</t>
+  </si>
+  <si>
+    <t>PvBHC7PUQB@gmail.com</t>
+  </si>
+  <si>
+    <t>UsvWPR9xTG@gmail.com</t>
+  </si>
+  <si>
+    <t>tLR4ipIRts@gmail.com</t>
+  </si>
+  <si>
+    <t>TnL6WtlKAP@gmail.com</t>
+  </si>
+  <si>
+    <t>LatffBkSAC@gmail.com</t>
+  </si>
+  <si>
+    <t>2pdphr5Dv1@gmail.com</t>
+  </si>
+  <si>
+    <t>h4C2a4FbwP@gmail.com</t>
+  </si>
+  <si>
+    <t>SVFQXIipsM@gmail.com</t>
+  </si>
+  <si>
+    <t>03SAbPSVXI@gmail.com</t>
+  </si>
+  <si>
+    <t>h3t4jBusDj@gmail.com</t>
+  </si>
+  <si>
+    <t>oWH3GVQutP@gmail.com</t>
+  </si>
+  <si>
+    <t>bDKfUIvwoI@gmail.com</t>
+  </si>
+  <si>
+    <t>X6xJPUfKte@gmail.com</t>
+  </si>
+  <si>
+    <t>Ks6feNRMGx@gmail.com</t>
+  </si>
+  <si>
+    <t>lmzQ032G0N@gmail.com</t>
+  </si>
+  <si>
+    <t>dM5vjoOZq1@gmail.com</t>
+  </si>
+  <si>
+    <t>3tYNcnwSnA@gmail.com</t>
+  </si>
+  <si>
+    <t>2ZAKadz4uQ@gmail.com</t>
+  </si>
+  <si>
+    <t>FYhMmoKpeo@gmail.com</t>
+  </si>
+  <si>
+    <t>oiszW1KfPg@gmail.com</t>
+  </si>
+  <si>
+    <t>ciWGUG7U5J@gmail.com</t>
+  </si>
+  <si>
+    <t>CzyxEJBUkX@gmail.com</t>
+  </si>
+  <si>
+    <t>YgtPGPDZhz@gmail.com</t>
+  </si>
+  <si>
+    <t>oi8o2m0LIJ@gmail.com</t>
+  </si>
+  <si>
+    <t>B3GKeFRdGa@gmail.com</t>
+  </si>
+  <si>
+    <t>fQOWYa980x@gmail.com</t>
+  </si>
+  <si>
+    <t>VmXtW1936c@gmail.com</t>
+  </si>
+  <si>
+    <t>Ldj8GZi6ja@gmail.com</t>
+  </si>
+  <si>
+    <t>Ib7kW5zj0u@gmail.com</t>
+  </si>
+  <si>
+    <t>HRzSWz3NBH@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -477,7 +723,7 @@
         <v>5536974644</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="F2" s="0">
         <v>23092001</v>

</xml_diff>